<commit_message>
[UPDATE] Adicionei verificacoes de erros, e ja comecei a colcoar as funcoes de calcular a ultima nota
</commit_message>
<xml_diff>
--- a/planilha_combinada.xlsx
+++ b/planilha_combinada.xlsx
@@ -428,6 +428,12 @@
       <c r="C2" t="str">
         <v>10</v>
       </c>
+      <c r="D2" t="str">
+        <v>29.5</v>
+      </c>
+      <c r="E2" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -439,6 +445,12 @@
       <c r="C3" t="str">
         <v>10</v>
       </c>
+      <c r="D3" t="str">
+        <v>29.5</v>
+      </c>
+      <c r="E3" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -450,6 +462,12 @@
       <c r="C4" t="str">
         <v>10</v>
       </c>
+      <c r="D4" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E4" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -461,6 +479,12 @@
       <c r="C5" t="str">
         <v>10</v>
       </c>
+      <c r="D5" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E5" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -472,6 +496,12 @@
       <c r="C6" t="str">
         <v>9.8</v>
       </c>
+      <c r="D6" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -483,6 +513,12 @@
       <c r="C7" t="str">
         <v>10</v>
       </c>
+      <c r="D7" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E7" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -494,6 +530,12 @@
       <c r="C8" t="str">
         <v>10</v>
       </c>
+      <c r="D8" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -505,6 +547,12 @@
       <c r="C9" t="str">
         <v>10</v>
       </c>
+      <c r="D9" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -516,6 +564,12 @@
       <c r="C10" t="str">
         <v>10</v>
       </c>
+      <c r="D10" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E10" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -527,6 +581,12 @@
       <c r="C11" t="str">
         <v>10</v>
       </c>
+      <c r="D11" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E11" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -538,6 +598,12 @@
       <c r="C12" t="str">
         <v>9.8</v>
       </c>
+      <c r="D12" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E12" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -549,6 +615,12 @@
       <c r="C13" t="str">
         <v>9.8</v>
       </c>
+      <c r="D13" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -560,6 +632,12 @@
       <c r="C14" t="str">
         <v>10</v>
       </c>
+      <c r="D14" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E14" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -571,6 +649,12 @@
       <c r="C15" t="str">
         <v>10</v>
       </c>
+      <c r="D15" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E15" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -582,6 +666,12 @@
       <c r="C16" t="str">
         <v>10</v>
       </c>
+      <c r="D16" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -593,6 +683,12 @@
       <c r="C17" t="str">
         <v>9.8</v>
       </c>
+      <c r="D17" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E17" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -604,6 +700,12 @@
       <c r="C18" t="str">
         <v>10</v>
       </c>
+      <c r="D18" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -615,6 +717,12 @@
       <c r="C19" t="str">
         <v>10</v>
       </c>
+      <c r="D19" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -626,6 +734,12 @@
       <c r="C20" t="str">
         <v>10</v>
       </c>
+      <c r="D20" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E20" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -637,6 +751,12 @@
       <c r="C21" t="str">
         <v>9.5</v>
       </c>
+      <c r="D21" t="str">
+        <v>28.5</v>
+      </c>
+      <c r="E21" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -648,6 +768,12 @@
       <c r="C22" t="str">
         <v>9.8</v>
       </c>
+      <c r="D22" t="str">
+        <v>29.6</v>
+      </c>
+      <c r="E22" t="str">
+        <v>4.1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -659,6 +785,12 @@
       <c r="C23" t="str">
         <v>10</v>
       </c>
+      <c r="D23" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E23" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -670,6 +802,12 @@
       <c r="C24" t="str">
         <v>10</v>
       </c>
+      <c r="D24" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E24" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -681,6 +819,12 @@
       <c r="C25" t="str">
         <v>9.8</v>
       </c>
+      <c r="D25" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E25" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -691,6 +835,12 @@
       </c>
       <c r="C26" t="str">
         <v>9.8</v>
+      </c>
+      <c r="D26" t="str">
+        <v>29.6</v>
+      </c>
+      <c r="E26" t="str">
+        <v>4.1</v>
       </c>
     </row>
   </sheetData>
@@ -725,6 +875,12 @@
       <c r="C2" t="str">
         <v>8.7</v>
       </c>
+      <c r="D2" t="str">
+        <v>25.2</v>
+      </c>
+      <c r="E2" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -736,6 +892,12 @@
       <c r="C3" t="str">
         <v>6.4</v>
       </c>
+      <c r="D3" t="str">
+        <v>20.3</v>
+      </c>
+      <c r="E3" t="str">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -747,6 +909,12 @@
       <c r="C4" t="str">
         <v>7.8</v>
       </c>
+      <c r="D4" t="str">
+        <v>24.0</v>
+      </c>
+      <c r="E4" t="str">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -758,6 +926,12 @@
       <c r="C5" t="str">
         <v>7.5</v>
       </c>
+      <c r="D5" t="str">
+        <v>23.3</v>
+      </c>
+      <c r="E5" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -769,6 +943,12 @@
       <c r="C6" t="str">
         <v>8.5</v>
       </c>
+      <c r="D6" t="str">
+        <v>26.2</v>
+      </c>
+      <c r="E6" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -780,6 +960,12 @@
       <c r="C7" t="str">
         <v>8</v>
       </c>
+      <c r="D7" t="str">
+        <v>23.5</v>
+      </c>
+      <c r="E7" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -791,6 +977,12 @@
       <c r="C8" t="str">
         <v>7.2</v>
       </c>
+      <c r="D8" t="str">
+        <v>21.0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -802,6 +994,12 @@
       <c r="C9" t="str">
         <v>8.6</v>
       </c>
+      <c r="D9" t="str">
+        <v>25.6</v>
+      </c>
+      <c r="E9" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -813,6 +1011,12 @@
       <c r="C10" t="str">
         <v>7.6</v>
       </c>
+      <c r="D10" t="str">
+        <v>24.0</v>
+      </c>
+      <c r="E10" t="str">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -824,6 +1028,12 @@
       <c r="C11" t="str">
         <v>5.8</v>
       </c>
+      <c r="D11" t="str">
+        <v>18.2</v>
+      </c>
+      <c r="E11" t="str">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -835,6 +1045,12 @@
       <c r="C12" t="str">
         <v>7</v>
       </c>
+      <c r="D12" t="str">
+        <v>21.5</v>
+      </c>
+      <c r="E12" t="str">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -846,6 +1062,12 @@
       <c r="C13" t="str">
         <v>9.2</v>
       </c>
+      <c r="D13" t="str">
+        <v>26.4</v>
+      </c>
+      <c r="E13" t="str">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -857,6 +1079,12 @@
       <c r="C14" t="str">
         <v>8.1</v>
       </c>
+      <c r="D14" t="str">
+        <v>24.7</v>
+      </c>
+      <c r="E14" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -868,6 +1096,12 @@
       <c r="C15" t="str">
         <v>8.1</v>
       </c>
+      <c r="D15" t="str">
+        <v>24.9</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -879,6 +1113,12 @@
       <c r="C16" t="str">
         <v>9</v>
       </c>
+      <c r="D16" t="str">
+        <v>27.1</v>
+      </c>
+      <c r="E16" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -890,6 +1130,12 @@
       <c r="C17" t="str">
         <v>6.5</v>
       </c>
+      <c r="D17" t="str">
+        <v>20.7</v>
+      </c>
+      <c r="E17" t="str">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -901,6 +1147,12 @@
       <c r="C18" t="str">
         <v>8.4</v>
       </c>
+      <c r="D18" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -912,6 +1164,12 @@
       <c r="C19" t="str">
         <v>8</v>
       </c>
+      <c r="D19" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E19" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -923,6 +1181,12 @@
       <c r="C20" t="str">
         <v>8.4</v>
       </c>
+      <c r="D20" t="str">
+        <v>24.3</v>
+      </c>
+      <c r="E20" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -934,6 +1198,12 @@
       <c r="C21" t="str">
         <v>7.4</v>
       </c>
+      <c r="D21" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E21" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -945,6 +1215,12 @@
       <c r="C22" t="str">
         <v>7.3</v>
       </c>
+      <c r="D22" t="str">
+        <v>22.4</v>
+      </c>
+      <c r="E22" t="str">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -956,6 +1232,12 @@
       <c r="C23" t="str">
         <v>7.4</v>
       </c>
+      <c r="D23" t="str">
+        <v>22.1</v>
+      </c>
+      <c r="E23" t="str">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -967,6 +1249,12 @@
       <c r="C24" t="str">
         <v>8.3</v>
       </c>
+      <c r="D24" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -978,6 +1266,12 @@
       <c r="C25" t="str">
         <v>8</v>
       </c>
+      <c r="D25" t="str">
+        <v>23.6</v>
+      </c>
+      <c r="E25" t="str">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -988,6 +1282,12 @@
       </c>
       <c r="C26" t="str">
         <v>7.9</v>
+      </c>
+      <c r="D26" t="str">
+        <v>23.1</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
@@ -1022,6 +1322,12 @@
       <c r="C2" t="str">
         <v>7.8</v>
       </c>
+      <c r="D2" t="str">
+        <v>23.8</v>
+      </c>
+      <c r="E2" t="str">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -1033,6 +1339,12 @@
       <c r="C3" t="str">
         <v>-</v>
       </c>
+      <c r="D3" t="str">
+        <v>NaN</v>
+      </c>
+      <c r="E3" t="str">
+        <v>NaN</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1044,6 +1356,12 @@
       <c r="C4" t="str">
         <v>8.3</v>
       </c>
+      <c r="D4" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E4" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1055,6 +1373,12 @@
       <c r="C5" t="str">
         <v>8.7</v>
       </c>
+      <c r="D5" t="str">
+        <v>26.1</v>
+      </c>
+      <c r="E5" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1066,6 +1390,12 @@
       <c r="C6" t="str">
         <v>8.7</v>
       </c>
+      <c r="D6" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1077,6 +1407,12 @@
       <c r="C7" t="str">
         <v>6.6</v>
       </c>
+      <c r="D7" t="str">
+        <v>20.3</v>
+      </c>
+      <c r="E7" t="str">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1088,6 +1424,12 @@
       <c r="C8" t="str">
         <v>6.3</v>
       </c>
+      <c r="D8" t="str">
+        <v>20.0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1099,6 +1441,12 @@
       <c r="C9" t="str">
         <v>9.7</v>
       </c>
+      <c r="D9" t="str">
+        <v>28.6</v>
+      </c>
+      <c r="E9" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1110,6 +1458,12 @@
       <c r="C10" t="str">
         <v>9.5</v>
       </c>
+      <c r="D10" t="str">
+        <v>28.1</v>
+      </c>
+      <c r="E10" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1121,6 +1475,12 @@
       <c r="C11" t="str">
         <v>5.1</v>
       </c>
+      <c r="D11" t="str">
+        <v>17.4</v>
+      </c>
+      <c r="E11" t="str">
+        <v>8.2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1132,6 +1492,12 @@
       <c r="C12" t="str">
         <v>6.5</v>
       </c>
+      <c r="D12" t="str">
+        <v>20.3</v>
+      </c>
+      <c r="E12" t="str">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1143,6 +1509,12 @@
       <c r="C13" t="str">
         <v>8.8</v>
       </c>
+      <c r="D13" t="str">
+        <v>27.1</v>
+      </c>
+      <c r="E13" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1154,6 +1526,12 @@
       <c r="C14" t="str">
         <v>8.1</v>
       </c>
+      <c r="D14" t="str">
+        <v>24.6</v>
+      </c>
+      <c r="E14" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1165,6 +1543,12 @@
       <c r="C15" t="str">
         <v>8.5</v>
       </c>
+      <c r="D15" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1176,6 +1560,12 @@
       <c r="C16" t="str">
         <v>9.5</v>
       </c>
+      <c r="D16" t="str">
+        <v>28.6</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1187,6 +1577,12 @@
       <c r="C17" t="str">
         <v>7.8</v>
       </c>
+      <c r="D17" t="str">
+        <v>23.0</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1198,6 +1594,12 @@
       <c r="C18" t="str">
         <v>8.8</v>
       </c>
+      <c r="D18" t="str">
+        <v>26.6</v>
+      </c>
+      <c r="E18" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1209,6 +1611,12 @@
       <c r="C19" t="str">
         <v>9</v>
       </c>
+      <c r="D19" t="str">
+        <v>26.2</v>
+      </c>
+      <c r="E19" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1220,6 +1628,12 @@
       <c r="C20" t="str">
         <v>7.5</v>
       </c>
+      <c r="D20" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1231,6 +1645,12 @@
       <c r="C21" t="str">
         <v>7.1</v>
       </c>
+      <c r="D21" t="str">
+        <v>21.6</v>
+      </c>
+      <c r="E21" t="str">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1242,6 +1662,12 @@
       <c r="C22" t="str">
         <v>8.3</v>
       </c>
+      <c r="D22" t="str">
+        <v>24.9</v>
+      </c>
+      <c r="E22" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1253,6 +1679,12 @@
       <c r="C23" t="str">
         <v>7.5</v>
       </c>
+      <c r="D23" t="str">
+        <v>22.8</v>
+      </c>
+      <c r="E23" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1264,6 +1696,12 @@
       <c r="C24" t="str">
         <v>9</v>
       </c>
+      <c r="D24" t="str">
+        <v>27.0</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1275,6 +1713,12 @@
       <c r="C25" t="str">
         <v>7</v>
       </c>
+      <c r="D25" t="str">
+        <v>22.1</v>
+      </c>
+      <c r="E25" t="str">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1285,6 +1729,12 @@
       </c>
       <c r="C26" t="str">
         <v>7.5</v>
+      </c>
+      <c r="D26" t="str">
+        <v>23.0</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
@@ -1319,6 +1769,12 @@
       <c r="C2" t="str">
         <v>9.4</v>
       </c>
+      <c r="D2" t="str">
+        <v>28.4</v>
+      </c>
+      <c r="E2" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -1330,6 +1786,12 @@
       <c r="C3" t="str">
         <v>8.1</v>
       </c>
+      <c r="D3" t="str">
+        <v>26.2</v>
+      </c>
+      <c r="E3" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1341,6 +1803,12 @@
       <c r="C4" t="str">
         <v>9.5</v>
       </c>
+      <c r="D4" t="str">
+        <v>28.2</v>
+      </c>
+      <c r="E4" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1352,6 +1820,12 @@
       <c r="C5" t="str">
         <v>9.8</v>
       </c>
+      <c r="D5" t="str">
+        <v>28.9</v>
+      </c>
+      <c r="E5" t="str">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1363,6 +1837,12 @@
       <c r="C6" t="str">
         <v>10</v>
       </c>
+      <c r="D6" t="str">
+        <v>29.6</v>
+      </c>
+      <c r="E6" t="str">
+        <v>4.1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1374,6 +1854,12 @@
       <c r="C7" t="str">
         <v>9.4</v>
       </c>
+      <c r="D7" t="str">
+        <v>27.6</v>
+      </c>
+      <c r="E7" t="str">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1385,6 +1871,12 @@
       <c r="C8" t="str">
         <v>8</v>
       </c>
+      <c r="D8" t="str">
+        <v>22.8</v>
+      </c>
+      <c r="E8" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1396,6 +1888,12 @@
       <c r="C9" t="str">
         <v>8.4</v>
       </c>
+      <c r="D9" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1407,6 +1905,12 @@
       <c r="C10" t="str">
         <v>10</v>
       </c>
+      <c r="D10" t="str">
+        <v>29.4</v>
+      </c>
+      <c r="E10" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1418,6 +1922,12 @@
       <c r="C11" t="str">
         <v>8.4</v>
       </c>
+      <c r="D11" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E11" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1429,6 +1939,12 @@
       <c r="C12" t="str">
         <v>7.6</v>
       </c>
+      <c r="D12" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E12" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1440,6 +1956,12 @@
       <c r="C13" t="str">
         <v>9.6</v>
       </c>
+      <c r="D13" t="str">
+        <v>28.4</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1451,6 +1973,12 @@
       <c r="C14" t="str">
         <v>8.8</v>
       </c>
+      <c r="D14" t="str">
+        <v>26.6</v>
+      </c>
+      <c r="E14" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1462,6 +1990,12 @@
       <c r="C15" t="str">
         <v>8.7</v>
       </c>
+      <c r="D15" t="str">
+        <v>26.1</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1473,6 +2007,12 @@
       <c r="C16" t="str">
         <v>9.4</v>
       </c>
+      <c r="D16" t="str">
+        <v>27.9</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1484,6 +2024,12 @@
       <c r="C17" t="str">
         <v>7.9</v>
       </c>
+      <c r="D17" t="str">
+        <v>23.5</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1495,6 +2041,12 @@
       <c r="C18" t="str">
         <v>10</v>
       </c>
+      <c r="D18" t="str">
+        <v>29.5</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1506,6 +2058,12 @@
       <c r="C19" t="str">
         <v>9</v>
       </c>
+      <c r="D19" t="str">
+        <v>27.4</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1517,6 +2075,12 @@
       <c r="C20" t="str">
         <v>9.2</v>
       </c>
+      <c r="D20" t="str">
+        <v>26.5</v>
+      </c>
+      <c r="E20" t="str">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1528,6 +2092,12 @@
       <c r="C21" t="str">
         <v>9</v>
       </c>
+      <c r="D21" t="str">
+        <v>28.0</v>
+      </c>
+      <c r="E21" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1539,6 +2109,12 @@
       <c r="C22" t="str">
         <v>8.7</v>
       </c>
+      <c r="D22" t="str">
+        <v>25.9</v>
+      </c>
+      <c r="E22" t="str">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1550,6 +2126,12 @@
       <c r="C23" t="str">
         <v>7.4</v>
       </c>
+      <c r="D23" t="str">
+        <v>22.7</v>
+      </c>
+      <c r="E23" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1561,6 +2143,12 @@
       <c r="C24" t="str">
         <v>10</v>
       </c>
+      <c r="D24" t="str">
+        <v>29.5</v>
+      </c>
+      <c r="E24" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1572,6 +2160,12 @@
       <c r="C25" t="str">
         <v>8.8</v>
       </c>
+      <c r="D25" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1582,6 +2176,12 @@
       </c>
       <c r="C26" t="str">
         <v>7.6</v>
+      </c>
+      <c r="D26" t="str">
+        <v>24.0</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -1616,6 +2216,12 @@
       <c r="C2" t="str">
         <v>7.9</v>
       </c>
+      <c r="D2" t="str">
+        <v>24.2</v>
+      </c>
+      <c r="E2" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -1627,6 +2233,12 @@
       <c r="C3" t="str">
         <v>8.2</v>
       </c>
+      <c r="D3" t="str">
+        <v>25.9</v>
+      </c>
+      <c r="E3" t="str">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1638,6 +2250,12 @@
       <c r="C4" t="str">
         <v>9.4</v>
       </c>
+      <c r="D4" t="str">
+        <v>28.4</v>
+      </c>
+      <c r="E4" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1649,6 +2267,12 @@
       <c r="C5" t="str">
         <v>8.7</v>
       </c>
+      <c r="D5" t="str">
+        <v>25.4</v>
+      </c>
+      <c r="E5" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1660,6 +2284,12 @@
       <c r="C6" t="str">
         <v>8.8</v>
       </c>
+      <c r="D6" t="str">
+        <v>26.8</v>
+      </c>
+      <c r="E6" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1671,6 +2301,12 @@
       <c r="C7" t="str">
         <v>7.6</v>
       </c>
+      <c r="D7" t="str">
+        <v>22.7</v>
+      </c>
+      <c r="E7" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1682,6 +2318,12 @@
       <c r="C8" t="str">
         <v>6.5</v>
       </c>
+      <c r="D8" t="str">
+        <v>19.0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1693,6 +2335,12 @@
       <c r="C9" t="str">
         <v>8.3</v>
       </c>
+      <c r="D9" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1704,6 +2352,12 @@
       <c r="C10" t="str">
         <v>7.6</v>
       </c>
+      <c r="D10" t="str">
+        <v>23.3</v>
+      </c>
+      <c r="E10" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1715,6 +2369,12 @@
       <c r="C11" t="str">
         <v>5</v>
       </c>
+      <c r="D11" t="str">
+        <v>17.3</v>
+      </c>
+      <c r="E11" t="str">
+        <v>8.2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1726,6 +2386,12 @@
       <c r="C12" t="str">
         <v>6.5</v>
       </c>
+      <c r="D12" t="str">
+        <v>21.2</v>
+      </c>
+      <c r="E12" t="str">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1737,6 +2403,12 @@
       <c r="C13" t="str">
         <v>9.8</v>
       </c>
+      <c r="D13" t="str">
+        <v>29.0</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1748,6 +2420,12 @@
       <c r="C14" t="str">
         <v>8.8</v>
       </c>
+      <c r="D14" t="str">
+        <v>26.1</v>
+      </c>
+      <c r="E14" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1759,6 +2437,12 @@
       <c r="C15" t="str">
         <v>8.9</v>
       </c>
+      <c r="D15" t="str">
+        <v>27.3</v>
+      </c>
+      <c r="E15" t="str">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1770,6 +2454,12 @@
       <c r="C16" t="str">
         <v>9.2</v>
       </c>
+      <c r="D16" t="str">
+        <v>28.1</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1781,6 +2471,12 @@
       <c r="C17" t="str">
         <v>7.3</v>
       </c>
+      <c r="D17" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1792,6 +2488,12 @@
       <c r="C18" t="str">
         <v>9.5</v>
       </c>
+      <c r="D18" t="str">
+        <v>28.4</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1803,6 +2505,12 @@
       <c r="C19" t="str">
         <v>9.4</v>
       </c>
+      <c r="D19" t="str">
+        <v>27.8</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1814,6 +2522,12 @@
       <c r="C20" t="str">
         <v>8.4</v>
       </c>
+      <c r="D20" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E20" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1825,6 +2539,12 @@
       <c r="C21" t="str">
         <v>9.5</v>
       </c>
+      <c r="D21" t="str">
+        <v>28.6</v>
+      </c>
+      <c r="E21" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1836,6 +2556,12 @@
       <c r="C22" t="str">
         <v>9.4</v>
       </c>
+      <c r="D22" t="str">
+        <v>27.5</v>
+      </c>
+      <c r="E22" t="str">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1847,6 +2573,12 @@
       <c r="C23" t="str">
         <v>7.7</v>
       </c>
+      <c r="D23" t="str">
+        <v>24.2</v>
+      </c>
+      <c r="E23" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1858,6 +2590,12 @@
       <c r="C24" t="str">
         <v>7.6</v>
       </c>
+      <c r="D24" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1869,6 +2607,12 @@
       <c r="C25" t="str">
         <v>9</v>
       </c>
+      <c r="D25" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1879,6 +2623,12 @@
       </c>
       <c r="C26" t="str">
         <v>7.3</v>
+      </c>
+      <c r="D26" t="str">
+        <v>22.6</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
@@ -1913,6 +2663,12 @@
       <c r="C2" t="str">
         <v>7.5</v>
       </c>
+      <c r="D2" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E2" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -1924,6 +2680,12 @@
       <c r="C3" t="str">
         <v>6.2</v>
       </c>
+      <c r="D3" t="str">
+        <v>21.4</v>
+      </c>
+      <c r="E3" t="str">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1935,6 +2697,12 @@
       <c r="C4" t="str">
         <v>7.2</v>
       </c>
+      <c r="D4" t="str">
+        <v>23.2</v>
+      </c>
+      <c r="E4" t="str">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1946,6 +2714,12 @@
       <c r="C5" t="str">
         <v>7</v>
       </c>
+      <c r="D5" t="str">
+        <v>22.8</v>
+      </c>
+      <c r="E5" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1957,6 +2731,12 @@
       <c r="C6" t="str">
         <v>8.7</v>
       </c>
+      <c r="D6" t="str">
+        <v>27.0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1968,6 +2748,12 @@
       <c r="C7" t="str">
         <v>7.3</v>
       </c>
+      <c r="D7" t="str">
+        <v>22.9</v>
+      </c>
+      <c r="E7" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1979,6 +2765,12 @@
       <c r="C8" t="str">
         <v>6.4</v>
       </c>
+      <c r="D8" t="str">
+        <v>20.1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1990,6 +2782,12 @@
       <c r="C9" t="str">
         <v>8.3</v>
       </c>
+      <c r="D9" t="str">
+        <v>25.6</v>
+      </c>
+      <c r="E9" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -2001,6 +2799,12 @@
       <c r="C10" t="str">
         <v>7.8</v>
       </c>
+      <c r="D10" t="str">
+        <v>24.6</v>
+      </c>
+      <c r="E10" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -2012,6 +2816,12 @@
       <c r="C11" t="str">
         <v>6</v>
       </c>
+      <c r="D11" t="str">
+        <v>19.3</v>
+      </c>
+      <c r="E11" t="str">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -2023,6 +2833,12 @@
       <c r="C12" t="str">
         <v>7</v>
       </c>
+      <c r="D12" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E12" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -2034,6 +2850,12 @@
       <c r="C13" t="str">
         <v>8.6</v>
       </c>
+      <c r="D13" t="str">
+        <v>26.7</v>
+      </c>
+      <c r="E13" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -2045,6 +2867,12 @@
       <c r="C14" t="str">
         <v>7.3</v>
       </c>
+      <c r="D14" t="str">
+        <v>23.6</v>
+      </c>
+      <c r="E14" t="str">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -2056,6 +2884,12 @@
       <c r="C15" t="str">
         <v>6.4</v>
       </c>
+      <c r="D15" t="str">
+        <v>21.4</v>
+      </c>
+      <c r="E15" t="str">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -2067,6 +2901,12 @@
       <c r="C16" t="str">
         <v>9.3</v>
       </c>
+      <c r="D16" t="str">
+        <v>28.2</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -2078,6 +2918,12 @@
       <c r="C17" t="str">
         <v>-</v>
       </c>
+      <c r="D17" t="str">
+        <v>NaN</v>
+      </c>
+      <c r="E17" t="str">
+        <v>NaN</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -2089,6 +2935,12 @@
       <c r="C18" t="str">
         <v>9.3</v>
       </c>
+      <c r="D18" t="str">
+        <v>27.9</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -2100,6 +2952,12 @@
       <c r="C19" t="str">
         <v>8.1</v>
       </c>
+      <c r="D19" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E19" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -2111,6 +2969,12 @@
       <c r="C20" t="str">
         <v>6.6</v>
       </c>
+      <c r="D20" t="str">
+        <v>22.0</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -2122,6 +2986,12 @@
       <c r="C21" t="str">
         <v>8.6</v>
       </c>
+      <c r="D21" t="str">
+        <v>26.3</v>
+      </c>
+      <c r="E21" t="str">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -2133,6 +3003,12 @@
       <c r="C22" t="str">
         <v>8</v>
       </c>
+      <c r="D22" t="str">
+        <v>25.0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -2144,6 +3020,12 @@
       <c r="C23" t="str">
         <v>7</v>
       </c>
+      <c r="D23" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E23" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -2155,6 +3037,12 @@
       <c r="C24" t="str">
         <v>9.4</v>
       </c>
+      <c r="D24" t="str">
+        <v>28.2</v>
+      </c>
+      <c r="E24" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -2166,6 +3054,12 @@
       <c r="C25" t="str">
         <v>8.2</v>
       </c>
+      <c r="D25" t="str">
+        <v>24.8</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -2176,6 +3070,12 @@
       </c>
       <c r="C26" t="str">
         <v>6.2</v>
+      </c>
+      <c r="D26" t="str">
+        <v>21.3</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>
@@ -2210,6 +3110,12 @@
       <c r="C2" t="str">
         <v>9</v>
       </c>
+      <c r="D2" t="str">
+        <v>27.1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -2221,6 +3127,12 @@
       <c r="C3" t="str">
         <v>9</v>
       </c>
+      <c r="D3" t="str">
+        <v>25.0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -2232,6 +3144,12 @@
       <c r="C4" t="str">
         <v>9.4</v>
       </c>
+      <c r="D4" t="str">
+        <v>27.6</v>
+      </c>
+      <c r="E4" t="str">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -2243,6 +3161,12 @@
       <c r="C5" t="str">
         <v>8.8</v>
       </c>
+      <c r="D5" t="str">
+        <v>26.6</v>
+      </c>
+      <c r="E5" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -2254,6 +3178,12 @@
       <c r="C6" t="str">
         <v>9.5</v>
       </c>
+      <c r="D6" t="str">
+        <v>28.6</v>
+      </c>
+      <c r="E6" t="str">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -2265,6 +3195,12 @@
       <c r="C7" t="str">
         <v>8.8</v>
       </c>
+      <c r="D7" t="str">
+        <v>25.1</v>
+      </c>
+      <c r="E7" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -2276,6 +3212,12 @@
       <c r="C8" t="str">
         <v>8.1</v>
       </c>
+      <c r="D8" t="str">
+        <v>23.9</v>
+      </c>
+      <c r="E8" t="str">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -2287,6 +3229,12 @@
       <c r="C9" t="str">
         <v>9</v>
       </c>
+      <c r="D9" t="str">
+        <v>26.6</v>
+      </c>
+      <c r="E9" t="str">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -2298,6 +3246,12 @@
       <c r="C10" t="str">
         <v>8.5</v>
       </c>
+      <c r="D10" t="str">
+        <v>24.8</v>
+      </c>
+      <c r="E10" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -2309,6 +3263,12 @@
       <c r="C11" t="str">
         <v>8</v>
       </c>
+      <c r="D11" t="str">
+        <v>23.0</v>
+      </c>
+      <c r="E11" t="str">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -2320,6 +3280,12 @@
       <c r="C12" t="str">
         <v>8.4</v>
       </c>
+      <c r="D12" t="str">
+        <v>23.3</v>
+      </c>
+      <c r="E12" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -2331,6 +3297,12 @@
       <c r="C13" t="str">
         <v>9.3</v>
       </c>
+      <c r="D13" t="str">
+        <v>27.9</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -2342,6 +3314,12 @@
       <c r="C14" t="str">
         <v>9</v>
       </c>
+      <c r="D14" t="str">
+        <v>25.5</v>
+      </c>
+      <c r="E14" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -2353,6 +3331,12 @@
       <c r="C15" t="str">
         <v>8.4</v>
       </c>
+      <c r="D15" t="str">
+        <v>24.9</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -2364,6 +3348,12 @@
       <c r="C16" t="str">
         <v>9.3</v>
       </c>
+      <c r="D16" t="str">
+        <v>27.6</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -2375,6 +3365,12 @@
       <c r="C17" t="str">
         <v>8.1</v>
       </c>
+      <c r="D17" t="str">
+        <v>23.4</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -2386,6 +3382,12 @@
       <c r="C18" t="str">
         <v>10</v>
       </c>
+      <c r="D18" t="str">
+        <v>29.1</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -2397,6 +3399,12 @@
       <c r="C19" t="str">
         <v>9.1</v>
       </c>
+      <c r="D19" t="str">
+        <v>27.2</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -2408,6 +3416,12 @@
       <c r="C20" t="str">
         <v>8.7</v>
       </c>
+      <c r="D20" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E20" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -2419,6 +3433,12 @@
       <c r="C21" t="str">
         <v>9</v>
       </c>
+      <c r="D21" t="str">
+        <v>27.8</v>
+      </c>
+      <c r="E21" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -2430,6 +3450,12 @@
       <c r="C22" t="str">
         <v>9</v>
       </c>
+      <c r="D22" t="str">
+        <v>25.0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -2441,6 +3467,12 @@
       <c r="C23" t="str">
         <v>8.6</v>
       </c>
+      <c r="D23" t="str">
+        <v>24.9</v>
+      </c>
+      <c r="E23" t="str">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -2452,6 +3484,12 @@
       <c r="C24" t="str">
         <v>8.8</v>
       </c>
+      <c r="D24" t="str">
+        <v>25.6</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -2463,6 +3501,12 @@
       <c r="C25" t="str">
         <v>8.6</v>
       </c>
+      <c r="D25" t="str">
+        <v>24.6</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -2473,6 +3517,12 @@
       </c>
       <c r="C26" t="str">
         <v>8</v>
+      </c>
+      <c r="D26" t="str">
+        <v>23.0</v>
+      </c>
+      <c r="E26" t="str">
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
@@ -2507,6 +3557,12 @@
       <c r="C2" t="str">
         <v>8.4</v>
       </c>
+      <c r="D2" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -2518,6 +3574,12 @@
       <c r="C3" t="str">
         <v>3.7</v>
       </c>
+      <c r="D3" t="str">
+        <v>15.2</v>
+      </c>
+      <c r="E3" t="str">
+        <v>8.9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -2529,6 +3591,12 @@
       <c r="C4" t="str">
         <v>7.9</v>
       </c>
+      <c r="D4" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E4" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -2540,6 +3608,12 @@
       <c r="C5" t="str">
         <v>8.6</v>
       </c>
+      <c r="D5" t="str">
+        <v>25.8</v>
+      </c>
+      <c r="E5" t="str">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -2551,6 +3625,12 @@
       <c r="C6" t="str">
         <v>8.7</v>
       </c>
+      <c r="D6" t="str">
+        <v>27.0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -2562,6 +3642,12 @@
       <c r="C7" t="str">
         <v>7</v>
       </c>
+      <c r="D7" t="str">
+        <v>20.5</v>
+      </c>
+      <c r="E7" t="str">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -2573,6 +3659,12 @@
       <c r="C8" t="str">
         <v>7.7</v>
       </c>
+      <c r="D8" t="str">
+        <v>22.5</v>
+      </c>
+      <c r="E8" t="str">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -2584,6 +3676,12 @@
       <c r="C9" t="str">
         <v>9.7</v>
       </c>
+      <c r="D9" t="str">
+        <v>28.8</v>
+      </c>
+      <c r="E9" t="str">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -2595,6 +3693,12 @@
       <c r="C10" t="str">
         <v>8.2</v>
       </c>
+      <c r="D10" t="str">
+        <v>25.6</v>
+      </c>
+      <c r="E10" t="str">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -2606,6 +3710,12 @@
       <c r="C11" t="str">
         <v>5.5</v>
       </c>
+      <c r="D11" t="str">
+        <v>18.4</v>
+      </c>
+      <c r="E11" t="str">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -2617,6 +3727,12 @@
       <c r="C12" t="str">
         <v>8.2</v>
       </c>
+      <c r="D12" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E12" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -2628,6 +3744,12 @@
       <c r="C13" t="str">
         <v>9.8</v>
       </c>
+      <c r="D13" t="str">
+        <v>29.4</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -2639,6 +3761,12 @@
       <c r="C14" t="str">
         <v>7.2</v>
       </c>
+      <c r="D14" t="str">
+        <v>23.6</v>
+      </c>
+      <c r="E14" t="str">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -2650,6 +3778,12 @@
       <c r="C15" t="str">
         <v>6.6</v>
       </c>
+      <c r="D15" t="str">
+        <v>21.6</v>
+      </c>
+      <c r="E15" t="str">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -2661,6 +3795,12 @@
       <c r="C16" t="str">
         <v>10</v>
       </c>
+      <c r="D16" t="str">
+        <v>29.3</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -2672,6 +3812,12 @@
       <c r="C17" t="str">
         <v>7.3</v>
       </c>
+      <c r="D17" t="str">
+        <v>22.1</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -2683,6 +3829,12 @@
       <c r="C18" t="str">
         <v>9.3</v>
       </c>
+      <c r="D18" t="str">
+        <v>27.8</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -2694,6 +3846,12 @@
       <c r="C19" t="str">
         <v>9.5</v>
       </c>
+      <c r="D19" t="str">
+        <v>27.8</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -2705,6 +3863,12 @@
       <c r="C20" t="str">
         <v>7</v>
       </c>
+      <c r="D20" t="str">
+        <v>21.2</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -2716,6 +3880,12 @@
       <c r="C21" t="str">
         <v>6.3</v>
       </c>
+      <c r="D21" t="str">
+        <v>21.7</v>
+      </c>
+      <c r="E21" t="str">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -2727,6 +3897,12 @@
       <c r="C22" t="str">
         <v>6.3</v>
       </c>
+      <c r="D22" t="str">
+        <v>19.0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -2738,6 +3914,12 @@
       <c r="C23" t="str">
         <v>7.9</v>
       </c>
+      <c r="D23" t="str">
+        <v>24.5</v>
+      </c>
+      <c r="E23" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -2749,6 +3931,12 @@
       <c r="C24" t="str">
         <v>8.6</v>
       </c>
+      <c r="D24" t="str">
+        <v>26.0</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -2760,6 +3948,12 @@
       <c r="C25" t="str">
         <v>7.9</v>
       </c>
+      <c r="D25" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -2770,6 +3964,12 @@
       </c>
       <c r="C26" t="str">
         <v>8.7</v>
+      </c>
+      <c r="D26" t="str">
+        <v>25.8</v>
+      </c>
+      <c r="E26" t="str">
+        <v>5.4</v>
       </c>
     </row>
   </sheetData>
@@ -2804,6 +4004,12 @@
       <c r="C2" t="str">
         <v>9.5</v>
       </c>
+      <c r="D2" t="str">
+        <v>28.1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>4.6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -2815,6 +4021,12 @@
       <c r="C3" t="str">
         <v>7</v>
       </c>
+      <c r="D3" t="str">
+        <v>20.6</v>
+      </c>
+      <c r="E3" t="str">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -2826,6 +4038,12 @@
       <c r="C4" t="str">
         <v>8.8</v>
       </c>
+      <c r="D4" t="str">
+        <v>26.1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -2837,6 +4055,12 @@
       <c r="C5" t="str">
         <v>7.6</v>
       </c>
+      <c r="D5" t="str">
+        <v>23.9</v>
+      </c>
+      <c r="E5" t="str">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -2848,6 +4072,12 @@
       <c r="C6" t="str">
         <v>10</v>
       </c>
+      <c r="D6" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -2859,6 +4089,12 @@
       <c r="C7" t="str">
         <v>8.2</v>
       </c>
+      <c r="D7" t="str">
+        <v>24.5</v>
+      </c>
+      <c r="E7" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -2870,6 +4106,12 @@
       <c r="C8" t="str">
         <v>9</v>
       </c>
+      <c r="D8" t="str">
+        <v>24.5</v>
+      </c>
+      <c r="E8" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -2881,6 +4123,12 @@
       <c r="C9" t="str">
         <v>10</v>
       </c>
+      <c r="D9" t="str">
+        <v>29.5</v>
+      </c>
+      <c r="E9" t="str">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -2892,6 +4140,12 @@
       <c r="C10" t="str">
         <v>9</v>
       </c>
+      <c r="D10" t="str">
+        <v>27.3</v>
+      </c>
+      <c r="E10" t="str">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -2903,6 +4157,12 @@
       <c r="C11" t="str">
         <v>5</v>
       </c>
+      <c r="D11" t="str">
+        <v>17.0</v>
+      </c>
+      <c r="E11" t="str">
+        <v>8.3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -2914,6 +4174,12 @@
       <c r="C12" t="str">
         <v>7.1</v>
       </c>
+      <c r="D12" t="str">
+        <v>22.6</v>
+      </c>
+      <c r="E12" t="str">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -2925,6 +4191,12 @@
       <c r="C13" t="str">
         <v>9.5</v>
       </c>
+      <c r="D13" t="str">
+        <v>29.0</v>
+      </c>
+      <c r="E13" t="str">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -2936,6 +4208,12 @@
       <c r="C14" t="str">
         <v>9.7</v>
       </c>
+      <c r="D14" t="str">
+        <v>28.9</v>
+      </c>
+      <c r="E14" t="str">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -2947,6 +4225,12 @@
       <c r="C15" t="str">
         <v>8.7</v>
       </c>
+      <c r="D15" t="str">
+        <v>25.1</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -2958,6 +4242,12 @@
       <c r="C16" t="str">
         <v>10</v>
       </c>
+      <c r="D16" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E16" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -2969,6 +4259,12 @@
       <c r="C17" t="str">
         <v>8.3</v>
       </c>
+      <c r="D17" t="str">
+        <v>24.4</v>
+      </c>
+      <c r="E17" t="str">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -2980,6 +4276,12 @@
       <c r="C18" t="str">
         <v>9.5</v>
       </c>
+      <c r="D18" t="str">
+        <v>28.0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -2991,6 +4293,12 @@
       <c r="C19" t="str">
         <v>10</v>
       </c>
+      <c r="D19" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -3002,6 +4310,12 @@
       <c r="C20" t="str">
         <v>7.5</v>
       </c>
+      <c r="D20" t="str">
+        <v>22.8</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -3013,6 +4327,12 @@
       <c r="C21" t="str">
         <v>7.7</v>
       </c>
+      <c r="D21" t="str">
+        <v>23.2</v>
+      </c>
+      <c r="E21" t="str">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -3024,6 +4344,12 @@
       <c r="C22" t="str">
         <v>7.5</v>
       </c>
+      <c r="D22" t="str">
+        <v>22.0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -3035,6 +4361,12 @@
       <c r="C23" t="str">
         <v>8.1</v>
       </c>
+      <c r="D23" t="str">
+        <v>24.7</v>
+      </c>
+      <c r="E23" t="str">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -3046,6 +4378,12 @@
       <c r="C24" t="str">
         <v>8</v>
       </c>
+      <c r="D24" t="str">
+        <v>24.0</v>
+      </c>
+      <c r="E24" t="str">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -3057,6 +4395,12 @@
       <c r="C25" t="str">
         <v>8.5</v>
       </c>
+      <c r="D25" t="str">
+        <v>25.3</v>
+      </c>
+      <c r="E25" t="str">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -3067,6 +4411,12 @@
       </c>
       <c r="C26" t="str">
         <v>8.8</v>
+      </c>
+      <c r="D26" t="str">
+        <v>25.6</v>
+      </c>
+      <c r="E26" t="str">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] Adicionais espacamento entre as colunas
</commit_message>
<xml_diff>
--- a/planilha_combinada.xlsx
+++ b/planilha_combinada.xlsx
@@ -409,6 +409,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -880,6 +888,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -1351,6 +1367,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -1822,6 +1846,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -2293,6 +2325,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -2764,6 +2804,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -3235,6 +3283,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -3706,6 +3762,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">
@@ -4177,6 +4241,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5">
       <c r="A5" t="str">

</xml_diff>